<commit_message>
Analizy IWRA i korelacje z elementami SSI
</commit_message>
<xml_diff>
--- a/pomocnicze/BibliografiaMendeley_tabela.xlsx
+++ b/pomocnicze/BibliografiaMendeley_tabela.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSZ\Desktop\STUDIA\doktorat_git\pomocnicze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A810713-D3DE-459C-96DA-B063EB6EB5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFEE606-4E3D-49AC-B888-65540213D211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-98" windowWidth="23183" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="-98" windowWidth="23243" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="20230615" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="224">
   <si>
     <t>Alves, H. (2010). Perceived value index in higher education. Innovative Marketing, 6(2), 33–42.</t>
   </si>
@@ -463,6 +464,240 @@
   </si>
   <si>
     <t>Zastempowski, M. (2013). Potencjał innowacyjny małych i średnich przedsiębiorstw na tle liderów polskiej gospodarki w świetle badań empirycznych. International Journal of Contemporary Management, 2013(Numer 12 (2)).</t>
+  </si>
+  <si>
+    <t>Aguillo, I. (2009). Measuring the institution’s footprint in the web. Library Hi Tech, 27(4), 540–556. https://doi.org/10.1108/073788309</t>
+  </si>
+  <si>
+    <t>Aguillo, I. (2023). Methodology of Ranking Web of Universities. Cybermetrics Lab. https://www.webometrics.info/en/Methodology</t>
+  </si>
+  <si>
+    <t>Alkuwaiti, A. (2021). Webometrics Ranking: Change in Methodology &amp; January 2021 Results at Glance. http://www.drahmedalkuwaiti.com/admin/data/form_14936/files/element_4_3f06cedca61fa7fbd8e20020e556832c-54-Change in Metho_Jan 2021 Result 210216.pdf</t>
+  </si>
+  <si>
+    <t>ARWU. (2022a). ARWU World University Ranking 2022. Ranking Shanghai. http://www.shanghairanking.com/rankings/arwu/2022</t>
+  </si>
+  <si>
+    <t>ARWU. (2022b). ARWU World University Rankings 2022 methodology. Ranking Shanghai. http://www.shanghairanking.com/methodology/arwu/2022</t>
+  </si>
+  <si>
+    <t>Athiyaman, A. (1997). Linking student satisfaction and service quality perceptions: the case of university education. European Journal of Marketing, 31(7), 528–540. https://doi.org/10.1108/03090569710176655</t>
+  </si>
+  <si>
+    <t>Beliczyński, J. (2011). Analiza systemu zarządzania wartością dla Klienta. W Przegląd problemów doskonalenia systemów zarządzania przedsiębiorstwem. Mfiles.pl.</t>
+  </si>
+  <si>
+    <t>Bielawa, A. (2011). Przegląd najważniejszych modeli zarządzania jakością usług. Studia i Prace WNEiZ, 24.</t>
+  </si>
+  <si>
+    <t>Bobińska, B. (2012). Funkcjonowanie sektora publicznego jako organizacji „otwartych na klienta”. Zeszyty Naukowe Zachodniopomorskiej Szkoły Biznesu Firma i Rynek, 1, 59–71.</t>
+  </si>
+  <si>
+    <t>Brady, M. K., &amp; Cronin, J. J. (2001). Some New Thoughts on Conceptualizing Perceived Service Quality: A Hierarchical Approach. Journal of Marketing, 65(3), 34–49. https://doi.org/10.1509/jmkg.65.3.34.18334</t>
+  </si>
+  <si>
+    <t>Bukowski, S., &amp; Kosmala, B. (2007). Techniki projekcyjne w identyfikacji przekonań. Psychoterapia, 4(143), 37–44. http://poradnia-empatia.pl/userfiles/poradnia-empatiapl/file/Techniki projekcyjne w identyfikacji przekonan po autoryzacji.pdf</t>
+  </si>
+  <si>
+    <t>Carroll, A. B. (1979). A three-dimensional conceptual model of corporate performance. Corporate Social Responsibility, 497–505. https://doi.org/10.5465/amr.1979.4498296</t>
+  </si>
+  <si>
+    <t>Clarkson, M. B. E. (1995). A Stakeholder Framework for Analyzing and Evaluating Corporate Social Performance. The Academy of Management Review, 20(1), 92. https://doi.org/10.2307/258888</t>
+  </si>
+  <si>
+    <t>Cronin, J. J. (2016). Retrospective: a cross-sectional test of the effect and conceptualization of service value revisited. Journal of Services Marketing, 30(3), 261–265. https://doi.org/10.1108/JSM-11-2015-0328</t>
+  </si>
+  <si>
+    <t>Cronin, J. J., Brady, M. K., Brand, R. R., Hightower, R., &amp; Shemwell, D. J. (1997). A cross‐sectional test of the effect and conceptualization of service value. Journal of Services Marketing, 11(6), 375–391. https://doi.org/10.1108/08876049710187482</t>
+  </si>
+  <si>
+    <t>Cybermetrics Lab. (2023). Ranking Web of Universities 2023. Webometrics 2023 Jan Ranking. https://www.webometrics.info/en/world</t>
+  </si>
+  <si>
+    <t>Czarnik, S., &amp; Turek, K. (2014). Aktywność zawodowa i wykształcenie Polaków. https://www.parp.gov.pl/images/PARP_publications/pdf/20012.pdf</t>
+  </si>
+  <si>
+    <t>ELA 2020. (2021). Ekonomiczne Losy Absolwentów - zbiór danych źródłowych dla Uczelni obejmujący dane absolwentów studiów I, II stopnia i jednolitych studiów magiserskich do 2020 roku. https://ela.nauka.gov.pl/pl/experts/source-data</t>
+  </si>
+  <si>
+    <t>Faishol, O. K. L. M. A., &amp; Subriadi, A. P. (2022). Change management scenario to improve Webometrics ranking. Procedia Computer Science, 197, 557–565. https://doi.org/10.1016/j.procs.2021.12.173</t>
+  </si>
+  <si>
+    <t>Freeman, R. E., &amp; McVea, J. (2001). A stakeholder approach to strategic management. SSRN Electronic Journal.</t>
+  </si>
+  <si>
+    <t>Gołata, K., &amp; Sojkin, B. (2020). Determinanty budowania wizerunku i reputacji wyższej uczelni wobec jej intersariuszy. Marketing Instytucji Naukowych i Badawczych, 35(1), 29–58. https://doi.org/10.2478/minib-2020-0002</t>
+  </si>
+  <si>
+    <t>Greszta, M. (2010). Pomiar efektywności: rynek. W Odpowiedzialny biznes 2010. Wydawnictwo HBRP.</t>
+  </si>
+  <si>
+    <t>Grudowski, P., &amp; Szefler, J. P. (2015). Stakeholders Satisfaction Index as an Important Factor of Improving Quality Management Systems of Universities in Poland. Managing in Recovering Markets, GCMRM 2015.</t>
+  </si>
+  <si>
+    <t>Gummesson, E. (1998). Productivity, quality and relationship marketing in service operations. International Journal of Contemporary Hospitality Management, 10(1), 4–15. https://doi.org/10.1108/09596119810199282</t>
+  </si>
+  <si>
+    <t>GUS. (2021). Rocznik Demograficzny. https://stat.gov.pl/download/gfx/portalinformacyjny/pl/defaultaktualnosci/5515/3/12/1/rocznik_demograficzny_2018.pdf</t>
+  </si>
+  <si>
+    <t>GUS. (2022). Ludność według cech społecznych – wyniki wstępne NSP 2021. https://stat.gov.pl/files/gfx/portalinformacyjny/pl/defaultaktualnosci/6494/2/1/1/ludnosc_wedlug_cech_spolecznych_-_wyniki_wstepne_nsp_2021.pdf</t>
+  </si>
+  <si>
+    <t>Hoonakker, P., &amp; Carayon, P. (2009). Questionnaire Survey Nonresponse: A Comparison of Postal Mail and Internet Surveys. International Journal of Human-Computer Interaction, 25(5), 348–373. https://doi.org/10.1080/10447310902864951</t>
+  </si>
+  <si>
+    <t>Iacobucci, D., Ostrom, A., &amp; Grayson, K. (1995). Distinguishing Service Quality and Customer Satisfaction: The Voice of the Consumer. Journal of Consumer Psychology, 4(3), 277–303. https://doi.org/10.1207/s15327663jcp0403_04</t>
+  </si>
+  <si>
+    <t>Jastrzębska, E. (2016). Angażowanie interesariuszy jako istota społecznej odpowiedzialności według ISO 26000. W Reklama i PR z perspektywy współczesnych problemów komunikacji marketingowej (Red.) A. Wiśniewska, A. Kozłowska (ss. 71–91). Wyższa Szkoła Promocji, Mediów i Show Businessu.</t>
+  </si>
+  <si>
+    <t>Kang, H., &amp; Ahn, J.-W. (2021). Model Setting and Interpretation of Results in Research Using Structural Equation Modeling: A Checklist with Guiding Questions for Reporting. Asian Nursing Research, 15(3), 157–162. https://doi.org/10.1016/j.anr.2021.06.001</t>
+  </si>
+  <si>
+    <t>Kapusta, M. (2019). Interesariusze – osoby, o których musisz pamiętać w projekcie. https://leadership-center.pl/blog/interesariusze-osoby-o-ktorych-musisz-pamietac-w-projekcie/</t>
+  </si>
+  <si>
+    <t>Karwacka, M. (2011). Interesariusze.</t>
+  </si>
+  <si>
+    <t>Khodayari, F., &amp; Khodayari, B. (2011). Service Quality in Higher Education (Case study: Measuring service quality of Islamic Azad University, Firoozkooh branch). Interdisciplinary Journal of Research in Business, 1(9), 38–46.</t>
+  </si>
+  <si>
+    <t>Khoo, S., Ha, H., &amp; McGregor, S. L. T. T. (2017). Service quality and student/customer satisfaction in the private tertiary education sector in Singapore. International Journal of Educational Management, 31(4), 430–444. https://doi.org/10.1108/IJEM-09-2015-0121</t>
+  </si>
+  <si>
+    <t>Kolman, R., &amp; Tkaczyk, T. (1996). Jakość usług. Poradnik. TNOiK.</t>
+  </si>
+  <si>
+    <t>Krosnick, J. A. (1999). SURVEY RESEARCH. Annual Review of Psychology, 50(1), 537–567. https://doi.org/10.1146/annurev.psych.50.1.537</t>
+  </si>
+  <si>
+    <t>Laloux, F. (2015). Pracować inaczej. Wydawnictwo Studio EMKA.</t>
+  </si>
+  <si>
+    <t>Likert, R. (1932). Technique for the Measurement of Attitudes. Archives of Psychology, 22(140).</t>
+  </si>
+  <si>
+    <t>Lisowska, A., &amp; Ziemiński, Ł. (2012). Zarządzanie jakością w urzędach administracji publicznej. Zeszyty Naukowe Uniwersytetu Przyrodniczo-Humanistycznego w Siedlcach, 95, 302–322.</t>
+  </si>
+  <si>
+    <t>Mainardes, E. W., Alves, H., &amp; Raposo, M. (2012). A model for stakeholder classification and stakeholder relationships. MANAGEMENT DECISION, 50(10), 1861–1879. https://doi.org/10.1108/00251741211279648</t>
+  </si>
+  <si>
+    <t>Matzat, U., Snijders, C., &amp; van der Horst, W. (2009). Effects of different types of progress indicators on drop-out rates in web surveys. Social Psychology, 40(1), 43.</t>
+  </si>
+  <si>
+    <t>MEiN. (2023). Ekonomiczne Losy Absolwentów. https://www.gov.pl/web/edukacja-i-nauka/ekonomiczne-losy-absolwentow</t>
+  </si>
+  <si>
+    <t>Mitchell, R. K., Agle, B. R., &amp; Wood, D. J. (1997). Towards a theory of stakeholder identification and Salience: Defining the Principle of Who and What Really Counts. Academy of Management, 22(4), 853–886.</t>
+  </si>
+  <si>
+    <t>Naukowiec.org. (2023). Siła korelacji, klasyfikacja - opis. https://www.naukowiec.org/wiedza/statystyka/sila-korelacji--klasyfikacja_512.html</t>
+  </si>
+  <si>
+    <t>Pawlikowski, J. M. (2010). Polskie uczelnie wobec wyzwań procesu Bolońskiego. Zespół Promotorów Bolońskich. http://health.bizcalcs.com/Calculator.asp?Calc=Frame-Size-Wrist</t>
+  </si>
+  <si>
+    <t>Perspektywy. (2022). Metodologia Rankingu Szkół Wyższych Perspektywy 2022. https://ranking.perspektywy.pl/2022/article/metodologia-rankingu-uczelni-akademickich-2022r</t>
+  </si>
+  <si>
+    <t>PN-EN ISO 9000:2015. (2016). Systemy zarządzania jakością - Podstawy i terminologia PN-EN ISO 9000.</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2020). Methodology of QS World University Rankings 2020. https://www.topuniversities.com/qs-world-university-rankings/methodology</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023a). Methodology of QS World University Rankings 2023. https://support.qs.com/hc/en-gb/articles/4405955370898-QS-World-University-Rankings</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023b). Methodology of QS WUR - Academic Reputation. https://support.qs.com/hc/en-gb/articles/4405952675346</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023c). Methodology of QS WUR - Citations Per Faculty Ratio. https://support.qs.com/hc/en-gb/articles/360019107580</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023d). Methodology of QS WUR - Employer Reputation. https://support.qs.com/hc/en-gb/articles/4407794203410</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023e). Methodology of QS WUR - Employment Outcomes. https://support.qs.com/hc/en-gb/articles/4744563188508</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023f). Methodology of QS WUR - Faculty-Sudent Ratio. https://support.qs.com/hc/en-gb/articles/360019108240</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023g). Methodology of QS WUR - Interantional Faculty Ratio. https://support.qs.com/hc/en-gb/articles/4403961809554</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023h). Methodology of QS WUR - International Research Network. https://support.qs.com/hc/en-gb/articles/360021865579</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023i). Methodology of QS WUR - International Students Ratio. https://support.qs.com/hc/en-gb/articles/4403961727506</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023j). Methodology of QS WUR - Sustainability. https://support.qs.com/hc/en-gb/articles/8322582098460</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023k). Methodology of QS WUR - Sustainability Ranking. https://support.qs.com/hc/en-gb/articles/6107352412828</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023l). Proposed Methodology of QS World University Rankings 2024. https://support.qs.com/hc/en-gb/articles/6478203732380-2024-Rankings-Cycle</t>
+  </si>
+  <si>
+    <t>QS Quacquarelli Symonds. (2023m). QS World University Rankings 2023. QS WUR Ranking. https://www.topuniversities.com/university-rankings/world-university-rankings/2023</t>
+  </si>
+  <si>
+    <t>Ramirez, R. (1999). Stakeholder analysis and conflict management. W Cultivating peace: conflict and collaboration in natural resource management. IDRC, Ottawa, ON, CA.</t>
+  </si>
+  <si>
+    <t>Rauhvargers, A. (2014). Where Are the Global Rankings Leading Us? An Analysis of Recent Methodological Changes and New Developments. European Journal of Education, 49(1), 29–44. https://doi.org/10.1111/ejed.12066</t>
+  </si>
+  <si>
+    <t>Spreng, R. A., &amp; Mackoy, R. D. (1996). An empirical examination of a model of perceived service quality and satisfaction. Journal of Retailing, 72(2), 201–214. https://doi.org/10.1016/S0022-4359(96)90014-7</t>
+  </si>
+  <si>
+    <t>Stoma, M. (2012). Modele i metody pomiaru jakości usług. http://www.qrpolska.pl/files/file/M3.pdf</t>
+  </si>
+  <si>
+    <t>Szefler, J. P., &amp; Zieliński, G. (2013). Doskonalenie jakości usług edukacyjnych poprzez ocenę wyniku działalności instytucji akademickiej (ss. 274–288). unknown.</t>
+  </si>
+  <si>
+    <t>Szymaniec-Mlicka, K. (2016). Zarządzanie relacjami z interesariuszami publicznych podmiotów leczniczych. Zeszyty Naukowe. Organizacja i Zarządzanie. Politechnika Śląska, 97(1964), 309–320.</t>
+  </si>
+  <si>
+    <t>Times Higher Education. (2022). World University Rankings 2023 methodology. Times Higher Education (THE) (Numer October 2022). https://www.timeshighereducation.com/sites/default/files/breaking_news_files/the_2023_world_university_rankings_methodology.pdf</t>
+  </si>
+  <si>
+    <t>Times Higher Education. (2023). THE World University Rankings 2023. THE WUR Ranking. https://www.timeshighereducation.com/world-university-rankings/2023/world-ranking</t>
+  </si>
+  <si>
+    <t>Townsend, P. (1995). Quality involves everyone: how Paul Revere discovered “quality has value”. Managing Service Quality: An International Journal, 5(2), 19–24. https://doi.org/10.1108/09604529510083549</t>
+  </si>
+  <si>
+    <t>Trzeciak, M. (2016). Analiza atrybutów interesariuszy projektu warunkujących sukces projektu. Zeszyty Naukowe. Organizacja i Zarządzanie / Politechnika Śląska, 89, 497–506. file:///C:/Users/JPSZ/Desktop/STUDIA/LITERATURA/interesariusze/Trzeciak_ZNOiZ_89_2016.pdf</t>
+  </si>
+  <si>
+    <t>Tutko, M. (2018). Assessment of the quality of internationalisation in higher education institutions. Studia Ekonomiczne, 361, 76–85.</t>
+  </si>
+  <si>
+    <t>Van Aswegen, A. S., &amp; Engelbrecht, A. S. (2009). The relationship between transformational leadership, integrity and an ethical climate in organizations. SA Journal of Human Resource Management, 7(1), 1–9.</t>
+  </si>
+  <si>
+    <t>Vehovar, V., Batagelj, Z., Manfreda, K. L., &amp; Zaletel, M. (2002). Nonresponse in web surveys. Survey nonresponse, 229–242.</t>
+  </si>
+  <si>
+    <t>Villar, A., Callegaro, M., &amp; Yang, Y. (2013). Where Am I? A Meta-Analysis of Experiments on the Effects of Progress Indicators for Web Surveys. Social Science Computer Review, 31(6), 744–762. https://doi.org/10.1177/0894439313497468</t>
+  </si>
+  <si>
+    <t>von Mises, L. (2006). Ekonomia i polityka: wykład elementarny. Fijorr Publishing.</t>
+  </si>
+  <si>
+    <t>Woźnicki, J. (2008). Legislacyjne określenie pozycji uczelni jako instytucji życia publicznego. W Społeczna odpowiedzialność uczelni (ss. 13–21). Wydawnictwo Politechniki Gdańskiej.</t>
+  </si>
+  <si>
+    <t>Zeithaml, V. A., Berry, L. L., &amp; Parasuraman, A. (1996). The Behavioral Consequences of Service Quality. Journal of Marketing, 60(2), 31–46. https://doi.org/10.1177/002224299606000203</t>
   </si>
 </sst>
 </file>
@@ -782,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+    <sheetView topLeftCell="A121" workbookViewId="0">
       <selection activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
@@ -1960,4 +2195,1779 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FEA447-EA32-469C-96EC-90E026FEAD1F}">
+  <dimension ref="A1:B220"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B222" sqref="B222"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A151">
+        <v>151</v>
+      </c>
+      <c r="B151" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A152">
+        <v>152</v>
+      </c>
+      <c r="B152" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A157">
+        <v>157</v>
+      </c>
+      <c r="B157" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A158">
+        <v>158</v>
+      </c>
+      <c r="B158" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A159">
+        <v>159</v>
+      </c>
+      <c r="B159" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A161">
+        <v>161</v>
+      </c>
+      <c r="B161" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A162">
+        <v>162</v>
+      </c>
+      <c r="B162" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A163">
+        <v>163</v>
+      </c>
+      <c r="B163" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A164">
+        <v>164</v>
+      </c>
+      <c r="B164" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A165">
+        <v>165</v>
+      </c>
+      <c r="B165" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A166">
+        <v>166</v>
+      </c>
+      <c r="B166" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A167">
+        <v>167</v>
+      </c>
+      <c r="B167" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A168">
+        <v>168</v>
+      </c>
+      <c r="B168" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A169">
+        <v>169</v>
+      </c>
+      <c r="B169" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A170">
+        <v>170</v>
+      </c>
+      <c r="B170" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A171">
+        <v>171</v>
+      </c>
+      <c r="B171" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A172">
+        <v>172</v>
+      </c>
+      <c r="B172" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A173">
+        <v>173</v>
+      </c>
+      <c r="B173" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A174">
+        <v>174</v>
+      </c>
+      <c r="B174" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A175">
+        <v>175</v>
+      </c>
+      <c r="B175" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A176">
+        <v>176</v>
+      </c>
+      <c r="B176" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A177">
+        <v>177</v>
+      </c>
+      <c r="B177" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A178">
+        <v>178</v>
+      </c>
+      <c r="B178" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A179">
+        <v>179</v>
+      </c>
+      <c r="B179" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A180">
+        <v>180</v>
+      </c>
+      <c r="B180" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A181">
+        <v>181</v>
+      </c>
+      <c r="B181" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A182">
+        <v>182</v>
+      </c>
+      <c r="B182" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A183">
+        <v>183</v>
+      </c>
+      <c r="B183" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A184">
+        <v>184</v>
+      </c>
+      <c r="B184" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A185">
+        <v>185</v>
+      </c>
+      <c r="B185" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A186">
+        <v>186</v>
+      </c>
+      <c r="B186" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A187">
+        <v>187</v>
+      </c>
+      <c r="B187" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A188">
+        <v>188</v>
+      </c>
+      <c r="B188" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A189">
+        <v>189</v>
+      </c>
+      <c r="B189" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A190">
+        <v>190</v>
+      </c>
+      <c r="B190" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A191">
+        <v>191</v>
+      </c>
+      <c r="B191" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A192">
+        <v>192</v>
+      </c>
+      <c r="B192" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A193">
+        <v>193</v>
+      </c>
+      <c r="B193" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A194">
+        <v>194</v>
+      </c>
+      <c r="B194" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A195">
+        <v>195</v>
+      </c>
+      <c r="B195" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A196">
+        <v>196</v>
+      </c>
+      <c r="B196" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A197">
+        <v>197</v>
+      </c>
+      <c r="B197" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A198">
+        <v>198</v>
+      </c>
+      <c r="B198" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A199">
+        <v>199</v>
+      </c>
+      <c r="B199" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="B200" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A201">
+        <v>201</v>
+      </c>
+      <c r="B201" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A202">
+        <v>202</v>
+      </c>
+      <c r="B202" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A203">
+        <v>203</v>
+      </c>
+      <c r="B203" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A204">
+        <v>204</v>
+      </c>
+      <c r="B204" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A205">
+        <v>205</v>
+      </c>
+      <c r="B205" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A206">
+        <v>206</v>
+      </c>
+      <c r="B206" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A207">
+        <v>207</v>
+      </c>
+      <c r="B207" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A208">
+        <v>208</v>
+      </c>
+      <c r="B208" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A209">
+        <v>209</v>
+      </c>
+      <c r="B209" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A210">
+        <v>210</v>
+      </c>
+      <c r="B210" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A211">
+        <v>211</v>
+      </c>
+      <c r="B211" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A212">
+        <v>212</v>
+      </c>
+      <c r="B212" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A213">
+        <v>213</v>
+      </c>
+      <c r="B213" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A214">
+        <v>214</v>
+      </c>
+      <c r="B214" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A215">
+        <v>215</v>
+      </c>
+      <c r="B215" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A216">
+        <v>216</v>
+      </c>
+      <c r="B216" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A217">
+        <v>217</v>
+      </c>
+      <c r="B217" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A218">
+        <v>218</v>
+      </c>
+      <c r="B218" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A219">
+        <v>219</v>
+      </c>
+      <c r="B219" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A220">
+        <v>220</v>
+      </c>
+      <c r="B220" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>